<commit_message>
Versión 0.753, Modificación de ejemplos y agregar método al Dosaje
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-RecetaCl.xlsx
+++ b/output/StructureDefinition-RecetaCl.xlsx
@@ -448,10 +448,10 @@
 requisition</t>
   </si>
   <si>
-    <t>Número identificador de grupo que debe ser el mismo con el cual se identificaron los farmacos prescritos en el acto clínico</t>
-  </si>
-  <si>
-    <t>Este numero vincula el contenedor con todos los farmacos prescritos durante la atención del paciente. Este hará el uso de Receta y el grupo de farmacos co misma identificacion grupal. El formato debe ser xxxxxxxx</t>
+    <t>Número identificador de grupo que debe ser el mismo con el cual se identificaron los farmacos prescritos en el acto clínico. El identificador debe ser un NanoId</t>
+  </si>
+  <si>
+    <t>Este numero vincula el contenedor con todos los farmacos prescritos durante la atención del paciente. Este hará el uso de Receta y el grupo de farmacos co misma identificacion grupal. El formato debe ser el de un NanoId</t>
   </si>
   <si>
     <t>Requests are linked either by a "basedOn" relationship (i.e. one request is fulfilling another) or by having a common requisition.  Requests that are part of the same requisition are generally treated independently from the perspective of changing their state or maintaining them after initial creation.</t>

</xml_diff>